<commit_message>
DRC 0 Errors, all footprint 3D correct
</commit_message>
<xml_diff>
--- a/Projects/OMD_CAN_F7_Ref/BOM/Bill of Materials-OMD_CAN_F7_REF.xlsx
+++ b/Projects/OMD_CAN_F7_Ref/BOM/Bill of Materials-OMD_CAN_F7_REF.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\OMD\OMD_Hardware\Projects\OMD_CAN_F7_Ref\BOM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="43170" windowHeight="22365"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="43170" windowHeight="22365" xr2:uid="{51AC7918-527F-46E7-A594-F23AAE7EEB27}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-OMD_CAN_F7_RE" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="340">
   <si>
     <t>Comment</t>
   </si>
@@ -74,6 +69,18 @@
     <t>Value</t>
   </si>
   <si>
+    <t>BATT</t>
+  </si>
+  <si>
+    <t>Socket</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>MOTOR_PLUG_F_3.5</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -98,6 +105,12 @@
     <t>24AC4318</t>
   </si>
   <si>
+    <t>Motor_pad</t>
+  </si>
+  <si>
+    <t>A, B, C</t>
+  </si>
+  <si>
     <t>DF40C-30-DS</t>
   </si>
   <si>
@@ -251,7 +264,7 @@
     <t>CAP, CERM, 1 µF, 6.3 V, +/- 10%, X7R, 0603</t>
   </si>
   <si>
-    <t>C8, C11, C47</t>
+    <t>C8, C11, C47, C53</t>
   </si>
   <si>
     <t>GRM188R70J105KA01D</t>
@@ -647,216 +660,201 @@
     <t>296-37194-1-ND</t>
   </si>
   <si>
-    <t>RES SMD 120 OHM 5% 1/16W 0402</t>
-  </si>
-  <si>
-    <t>R1_CAN1, R1_CAN2, R1_CAN3, R14_CAN1, R14_CAN2, R14_CAN3</t>
-  </si>
-  <si>
-    <t>R0402</t>
+    <t>RES SMD 10K OHM 5% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>R2, R8</t>
+  </si>
+  <si>
+    <t>0402-RES</t>
   </si>
   <si>
     <t>Resistor</t>
   </si>
   <si>
-    <t>RC0402JR-07120RL</t>
-  </si>
-  <si>
-    <t>311-120JRTR-ND</t>
+    <t>RC0402JR-0710KL</t>
+  </si>
+  <si>
+    <t>311-10KJRTR-ND</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>Current sense resistor</t>
+  </si>
+  <si>
+    <t>2W, 0.001R 5025 current sense resistor</t>
+  </si>
+  <si>
+    <t>R3_A, R3_B, R3_C</t>
+  </si>
+  <si>
+    <t>4RESC5125X09N</t>
+  </si>
+  <si>
+    <t>WSLP20101L000FEK</t>
+  </si>
+  <si>
+    <t>Stackpole Electronics Inc.</t>
+  </si>
+  <si>
+    <t>CSNL2010FT1L00</t>
+  </si>
+  <si>
+    <t>CSNL2010FT1L00CT-ND</t>
+  </si>
+  <si>
+    <t>0.001R</t>
+  </si>
+  <si>
+    <t>2K</t>
+  </si>
+  <si>
+    <t>RES 2K OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>R4, R5, R11, R12, R13</t>
+  </si>
+  <si>
+    <t>RESISTOR0402-RES</t>
+  </si>
+  <si>
+    <t>311-2.0KLRCT-ND</t>
+  </si>
+  <si>
+    <t>RES, 28.0 k, 1%, 0.1 W, 0603</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>0603L</t>
+  </si>
+  <si>
+    <t>CRCW060328K0FKEA</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>541-28.0KHCT-ND</t>
+  </si>
+  <si>
+    <t>28.0k</t>
+  </si>
+  <si>
+    <t>RES, 8.45 k, 1%, 0.1 W, 0603</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>CRCW06038K45FKEA</t>
+  </si>
+  <si>
+    <t>541-8.45KHCT-ND</t>
+  </si>
+  <si>
+    <t>8.45k</t>
+  </si>
+  <si>
+    <t>RES</t>
+  </si>
+  <si>
+    <t>RES SMD 18K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>R9_A, R9_B, R9_C, R16</t>
+  </si>
+  <si>
+    <t>R0805</t>
+  </si>
+  <si>
+    <t>R00155</t>
+  </si>
+  <si>
+    <t>RC0805FR-0718KL</t>
+  </si>
+  <si>
+    <t>311-18.0KCRCT-ND</t>
+  </si>
+  <si>
+    <t>18k</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>R10_A, R10_B, R10_C, R18</t>
+  </si>
+  <si>
+    <t>R00095</t>
+  </si>
+  <si>
+    <t>RC0805FR-071KL</t>
+  </si>
+  <si>
+    <t>311-1.00KCRCT-ND</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>PWR163</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PWR163 Series is a DPAK style surface mount power resistor. </t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>Resistor 25W 1R  DPAK</t>
+  </si>
+  <si>
+    <t>Bourns Inc.</t>
+  </si>
+  <si>
+    <t>PWR163S-25-1R00J</t>
+  </si>
+  <si>
+    <t>PWR163S-25-1R00J-ND</t>
+  </si>
+  <si>
+    <t>RES 10K OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>R19, R24</t>
+  </si>
+  <si>
+    <t>RC0402FR-0710KL</t>
+  </si>
+  <si>
+    <t>311-10.0KLRCT-ND</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>RES 1K OHM 1/16W 1% 0402</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics America, Inc.</t>
+  </si>
+  <si>
+    <t>RC1005F102CS</t>
+  </si>
+  <si>
+    <t>1276-3430-1-ND</t>
   </si>
   <si>
     <t>120R</t>
   </si>
   <si>
-    <t>RES SMD 10K OHM 5% 1/16W 0402</t>
-  </si>
-  <si>
-    <t>R2, R8</t>
-  </si>
-  <si>
-    <t>0402-RES</t>
-  </si>
-  <si>
-    <t>RC0402JR-0710KL</t>
-  </si>
-  <si>
-    <t>311-10KJRTR-ND</t>
-  </si>
-  <si>
-    <t>10K</t>
-  </si>
-  <si>
-    <t>Current sense resistor</t>
-  </si>
-  <si>
-    <t>2W, 0.001R 5025 current sense resistor</t>
-  </si>
-  <si>
-    <t>R3_A, R3_B, R3_C</t>
-  </si>
-  <si>
-    <t>4RESC5125X09N</t>
-  </si>
-  <si>
-    <t>WSLP20101L000FEK</t>
-  </si>
-  <si>
-    <t>Stackpole Electronics Inc.</t>
-  </si>
-  <si>
-    <t>CSNL2010FT1L00</t>
-  </si>
-  <si>
-    <t>CSNL2010FT1L00CT-ND</t>
-  </si>
-  <si>
-    <t>0.001R</t>
-  </si>
-  <si>
-    <t>2K</t>
-  </si>
-  <si>
-    <t>RES 2K OHM 1/16W 1% 0402 SMD</t>
-  </si>
-  <si>
-    <t>R4, R5, R11, R12, R13</t>
-  </si>
-  <si>
-    <t>RESISTOR0402-RES</t>
-  </si>
-  <si>
-    <t>311-2.0KLRCT-ND</t>
-  </si>
-  <si>
-    <t>RES, 28.0 k, 1%, 0.1 W, 0603</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>0603L</t>
-  </si>
-  <si>
-    <t>CRCW060328K0FKEA</t>
-  </si>
-  <si>
-    <t>Vishay Dale</t>
-  </si>
-  <si>
-    <t>541-28.0KHCT-ND</t>
-  </si>
-  <si>
-    <t>28.0k</t>
-  </si>
-  <si>
-    <t>RES, 8.45 k, 1%, 0.1 W, 0603</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>CRCW06038K45FKEA</t>
-  </si>
-  <si>
-    <t>541-8.45KHCT-ND</t>
-  </si>
-  <si>
-    <t>8.45k</t>
-  </si>
-  <si>
-    <t>RES</t>
-  </si>
-  <si>
-    <t>RES SMD 18K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>R9_A, R9_B, R9_C, R16</t>
-  </si>
-  <si>
-    <t>R0805</t>
-  </si>
-  <si>
-    <t>R00155</t>
-  </si>
-  <si>
-    <t>RC0805FR-0718KL</t>
-  </si>
-  <si>
-    <t>311-18.0KCRCT-ND</t>
-  </si>
-  <si>
-    <t>18k</t>
-  </si>
-  <si>
-    <t>RES SMD 1K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>R10_A, R10_B, R10_C, R18</t>
-  </si>
-  <si>
-    <t>R00095</t>
-  </si>
-  <si>
-    <t>RC0805FR-071KL</t>
-  </si>
-  <si>
-    <t>311-1.00KCRCT-ND</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t>1R2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ES SMD 1.2 OHM 5% 3W 2512  </t>
-  </si>
-  <si>
-    <t>R15</t>
-  </si>
-  <si>
-    <t>RESC6433X11N</t>
-  </si>
-  <si>
-    <t>TE Connectivity Passive Product</t>
-  </si>
-  <si>
-    <t>35221R2JT</t>
-  </si>
-  <si>
-    <t>A121178CT-ND</t>
-  </si>
-  <si>
-    <t>RES 10K OHM 1/16W 1% 0402 SMD</t>
-  </si>
-  <si>
-    <t>R19</t>
-  </si>
-  <si>
-    <t>RC0402FR-0710KL</t>
-  </si>
-  <si>
-    <t>311-10.0KLRCT-ND</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>RES 1K OHM 1/16W 1% 0402</t>
-  </si>
-  <si>
-    <t>R20</t>
-  </si>
-  <si>
-    <t>Samsung Electro-Mechanics America, Inc.</t>
-  </si>
-  <si>
-    <t>RC1005F102CS</t>
-  </si>
-  <si>
-    <t>1276-3430-1-ND</t>
-  </si>
-  <si>
     <t>RES 120 OHM 1/16W 1% 0402 SMD</t>
   </si>
   <si>
@@ -867,6 +865,27 @@
   </si>
   <si>
     <t>311-120LRCT-ND</t>
+  </si>
+  <si>
+    <t>0R</t>
+  </si>
+  <si>
+    <t>RES 0OHM 1/16W 1% 0201 SMD</t>
+  </si>
+  <si>
+    <t>R22, R23</t>
+  </si>
+  <si>
+    <t>0201-RES</t>
+  </si>
+  <si>
+    <t>Panasonic Electronic Components</t>
+  </si>
+  <si>
+    <t>ERJ-1GN0R00C</t>
+  </si>
+  <si>
+    <t>P15979TR-ND</t>
   </si>
   <si>
     <t>VL53L0X</t>
@@ -1025,7 +1044,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1413,12 +1432,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5BE604D-2C14-431C-BC2C-462E81021C20}">
+  <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1479,22 +1496,22 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>20</v>
@@ -1503,519 +1520,503 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="3">
-        <v>5000</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="K2" s="3"/>
       <c r="L2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="3">
-        <v>61</v>
-      </c>
-      <c r="N2" s="3">
-        <v>40250</v>
-      </c>
-      <c r="O2" s="3">
-        <v>8.0500000000000007</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
       <c r="P2" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="H3" s="3">
         <v>1</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K3" s="3">
         <v>5000</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="M3" s="3">
-        <v>4000</v>
+        <v>61</v>
       </c>
       <c r="N3" s="3">
-        <v>2696.90479</v>
+        <v>40250</v>
       </c>
       <c r="O3" s="3">
-        <v>0.53937999999999997</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H4" s="3">
         <v>3</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="M4" s="3">
-        <v>0</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="2" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="H5" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K5" s="3">
-        <v>20000</v>
+        <v>5000</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="M5" s="3">
-        <v>630000</v>
+        <v>4000</v>
       </c>
       <c r="N5" s="3">
-        <v>86.710279999999997</v>
+        <v>2563.2020200000002</v>
       </c>
       <c r="O5" s="3">
-        <v>4.3400000000000001E-3</v>
+        <v>0.51263999999999998</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="H6" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="3">
-        <v>5000</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="K6" s="3"/>
       <c r="L6" s="4" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="M6" s="3">
-        <v>32000</v>
-      </c>
-      <c r="N6" s="3">
-        <v>2680.7661600000001</v>
-      </c>
-      <c r="O6" s="3">
-        <v>0.53615000000000002</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
       <c r="P6" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H7" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K7" s="3">
-        <v>5000</v>
+        <v>20000</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="M7" s="3">
-        <v>127134</v>
+        <v>460000</v>
       </c>
       <c r="N7" s="3">
-        <v>329.38747999999998</v>
+        <v>82.367810000000006</v>
       </c>
       <c r="O7" s="3">
-        <v>6.5879999999999994E-2</v>
+        <v>4.1200000000000004E-3</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H8" s="3">
         <v>1</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K8" s="3">
         <v>5000</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="M8" s="3">
-        <v>1516</v>
+        <v>20000</v>
       </c>
       <c r="N8" s="3">
-        <v>1660.80465</v>
+        <v>2547.8473300000001</v>
       </c>
       <c r="O8" s="3">
-        <v>0.33216000000000001</v>
+        <v>0.50956999999999997</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H9" s="3">
         <v>1</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K9" s="3">
         <v>5000</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="M9" s="3">
-        <v>698274</v>
+        <v>104388</v>
       </c>
       <c r="N9" s="3">
-        <v>941.02167999999995</v>
+        <v>313.04527999999999</v>
       </c>
       <c r="O9" s="3">
-        <v>0.18820000000000001</v>
+        <v>6.2609999999999999E-2</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="H10" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K10" s="3">
-        <v>15000</v>
+        <v>5000</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M10" s="3">
-        <v>774</v>
+        <v>3506</v>
       </c>
       <c r="N10" s="3">
-        <v>1890.1326100000001</v>
+        <v>1578.4782299999999</v>
       </c>
       <c r="O10" s="3">
-        <v>0.12601000000000001</v>
+        <v>0.31569999999999998</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H11" s="3">
         <v>1</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K11" s="3">
         <v>5000</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="M11" s="3">
-        <v>11065</v>
+        <v>246</v>
       </c>
       <c r="N11" s="3">
-        <v>222.79281</v>
+        <v>894.38107000000002</v>
       </c>
       <c r="O11" s="3">
-        <v>4.4560000000000002E-2</v>
+        <v>0.17888000000000001</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>87</v>
+        <v>41</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="H12" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K12" s="3">
-        <v>5000</v>
+        <v>20000</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="M12" s="3">
         <v>0</v>
       </c>
       <c r="N12" s="3">
-        <v>629.28707999999995</v>
+        <v>4276.7777400000004</v>
       </c>
       <c r="O12" s="3">
-        <v>0.12586</v>
+        <v>0.21384</v>
       </c>
       <c r="P12" s="2" t="s">
         <v>84</v>
@@ -2023,1346 +2024,1346 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>93</v>
+        <v>41</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="H13" s="3">
         <v>1</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K13" s="3">
         <v>5000</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="M13" s="3">
-        <v>0</v>
+        <v>5845</v>
       </c>
       <c r="N13" s="3">
-        <v>2283.2377900000001</v>
+        <v>211.75192000000001</v>
       </c>
       <c r="O13" s="3">
-        <v>0.45665</v>
+        <v>4.2349999999999999E-2</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="H14" s="3">
         <v>1</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K14" s="3">
         <v>5000</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="M14" s="3">
-        <v>533725</v>
+        <v>0</v>
       </c>
       <c r="N14" s="3">
-        <v>87.467399999999998</v>
+        <v>598.07915000000003</v>
       </c>
       <c r="O14" s="3">
-        <v>1.7489999999999999E-2</v>
+        <v>0.11962</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>104</v>
+        <v>38</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="H15" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K15" s="3">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="M15" s="3">
-        <v>27796</v>
+        <v>0</v>
       </c>
       <c r="N15" s="3">
-        <v>726.59704999999997</v>
+        <v>2170.0504799999999</v>
       </c>
       <c r="O15" s="3">
-        <v>7.2660000000000002E-2</v>
+        <v>0.43401000000000001</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>41</v>
+        <v>103</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>110</v>
+        <v>58</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H16" s="3">
         <v>1</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K16" s="3">
         <v>5000</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="M16" s="3">
-        <v>1610559</v>
+        <v>511525</v>
       </c>
       <c r="N16" s="3">
-        <v>16.776209999999999</v>
+        <v>83.121650000000002</v>
       </c>
       <c r="O16" s="3">
-        <v>3.3600000000000001E-3</v>
+        <v>1.6619999999999999E-2</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>40</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="H17" s="3">
+        <v>2</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K17" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="H17" s="3">
-        <v>15</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K17" s="3">
-        <v>75000</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="M17" s="3">
-        <v>45000</v>
+        <v>39717</v>
       </c>
       <c r="N17" s="3">
-        <v>720.26115000000004</v>
+        <v>690.52471000000003</v>
       </c>
       <c r="O17" s="3">
-        <v>9.5999999999999992E-3</v>
+        <v>6.905E-2</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>16</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18" s="3">
+        <v>5000</v>
+      </c>
+      <c r="L18" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="H18" s="3">
-        <v>10</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K18" s="3">
-        <v>50000</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>123</v>
-      </c>
       <c r="M18" s="3">
-        <v>0</v>
+        <v>1604656</v>
       </c>
       <c r="N18" s="3">
-        <v>173500</v>
+        <v>15.94984</v>
       </c>
       <c r="O18" s="3">
-        <v>3.47</v>
+        <v>3.1900000000000001E-3</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>124</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>125</v>
+        <v>46</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H19" s="3">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K19" s="3">
-        <v>10000</v>
+        <v>75000</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="M19" s="3">
-        <v>31411</v>
+        <v>30000</v>
       </c>
       <c r="N19" s="3">
-        <v>28.770600000000002</v>
+        <v>684.41458</v>
       </c>
       <c r="O19" s="3">
-        <v>2.8800000000000002E-3</v>
+        <v>9.1299999999999992E-3</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H20" s="3">
+        <v>10</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" s="3">
+        <v>50000</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="M20" s="3">
+        <v>0</v>
+      </c>
+      <c r="N20" s="3">
+        <v>173500</v>
+      </c>
+      <c r="O20" s="3">
+        <v>3.47</v>
+      </c>
+      <c r="P20" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="H20" s="3">
-        <v>2</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K20" s="3">
-        <v>10000</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="M20" s="3">
-        <v>271315</v>
-      </c>
-      <c r="N20" s="3">
-        <v>4504.9495399999996</v>
-      </c>
-      <c r="O20" s="3">
-        <v>0.45049</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H21" s="3">
         <v>2</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K21" s="3">
         <v>10000</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="M21" s="3">
-        <v>721830</v>
+        <v>31411</v>
       </c>
       <c r="N21" s="3">
-        <v>564.65286000000003</v>
+        <v>27.376580000000001</v>
       </c>
       <c r="O21" s="3">
-        <v>5.6469999999999999E-2</v>
+        <v>2.7399999999999998E-3</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>66</v>
+        <v>136</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>139</v>
+        <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="H22" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K22" s="3">
         <v>10000</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="M22" s="3">
-        <v>0</v>
+        <v>404812</v>
       </c>
       <c r="N22" s="3">
-        <v>2112.1284500000002</v>
+        <v>4281.6182399999998</v>
       </c>
       <c r="O22" s="3">
-        <v>0.21121000000000001</v>
+        <v>0.42815999999999999</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>16</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H23" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K23" s="3">
         <v>10000</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="M23" s="3">
-        <v>110000</v>
+        <v>889138</v>
       </c>
       <c r="N23" s="3">
-        <v>1005.13788</v>
+        <v>536.66038000000003</v>
       </c>
       <c r="O23" s="3">
-        <v>0.10051</v>
+        <v>5.3670000000000002E-2</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>88</v>
+        <v>147</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H24" s="3">
         <v>1</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K24" s="3">
-        <v>15000</v>
+        <v>10000</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="M24" s="3">
-        <v>210000</v>
+        <v>0</v>
       </c>
       <c r="N24" s="3">
-        <v>274.35674</v>
+        <v>2007.3780300000001</v>
       </c>
       <c r="O24" s="3">
-        <v>1.8290000000000001E-2</v>
+        <v>0.20074</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="H25" s="3">
+        <v>1</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K25" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L25" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="H25" s="3">
-        <v>3</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K25" s="3">
-        <v>15000</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>158</v>
-      </c>
       <c r="M25" s="3">
-        <v>140000</v>
+        <v>290000</v>
       </c>
       <c r="N25" s="3">
-        <v>2769.3891600000002</v>
+        <v>955.32371999999998</v>
       </c>
       <c r="O25" s="3">
-        <v>0.18462999999999999</v>
+        <v>9.5530000000000004E-2</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>162</v>
+        <v>94</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>163</v>
+        <v>51</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="H26" s="3">
         <v>1</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K26" s="3">
-        <v>5000</v>
+        <v>15000</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="M26" s="3">
-        <v>1783</v>
+        <v>285000</v>
       </c>
       <c r="N26" s="3">
-        <v>2082.5210400000001</v>
+        <v>260.79171000000002</v>
       </c>
       <c r="O26" s="3">
-        <v>0.41649999999999998</v>
+        <v>1.7389999999999999E-2</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>165</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="F27" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G27" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="G27" s="4" t="s">
-        <v>171</v>
-      </c>
       <c r="H27" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K27" s="3">
-        <v>5000</v>
+        <v>15000</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="M27" s="3">
-        <v>141675</v>
+        <v>137500</v>
       </c>
       <c r="N27" s="3">
-        <v>325.60187000000002</v>
+        <v>2632.0799200000001</v>
       </c>
       <c r="O27" s="3">
-        <v>6.5119999999999997E-2</v>
+        <v>0.17546999999999999</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>173</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>174</v>
+        <v>38</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>45</v>
+        <v>169</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="H28" s="3">
         <v>1</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K28" s="3">
         <v>5000</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="M28" s="3">
-        <v>3596</v>
+        <v>0</v>
       </c>
       <c r="N28" s="3">
-        <v>837.77428999999995</v>
+        <v>1979.28728</v>
       </c>
       <c r="O28" s="3">
-        <v>0.16755</v>
+        <v>0.39585999999999999</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>73</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>32</v>
+        <v>172</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="H29" s="3">
         <v>1</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K29" s="3">
         <v>5000</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="M29" s="3">
-        <v>11916</v>
+        <v>136649</v>
       </c>
       <c r="N29" s="3">
-        <v>3724.2382699999998</v>
+        <v>309.47442000000001</v>
       </c>
       <c r="O29" s="3">
-        <v>0.74485000000000001</v>
+        <v>6.1890000000000001E-2</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>183</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>191</v>
+        <v>51</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="H30" s="3">
         <v>1</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K30" s="3">
         <v>5000</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="M30" s="3">
-        <v>400</v>
+        <v>42931</v>
       </c>
       <c r="N30" s="3">
-        <v>14727.11887</v>
+        <v>796.26180999999997</v>
       </c>
       <c r="O30" s="3">
-        <v>2.9454199999999999</v>
+        <v>0.15925</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>193</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>194</v>
+        <v>38</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>156</v>
+        <v>190</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="H31" s="3">
         <v>1</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K31" s="3">
         <v>5000</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="M31" s="3">
-        <v>0</v>
+        <v>11878</v>
       </c>
       <c r="N31" s="3">
-        <v>2362.8550399999999</v>
+        <v>5375.1738699999996</v>
       </c>
       <c r="O31" s="3">
-        <v>0.47256999999999999</v>
+        <v>1.0750299999999999</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>16</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="H32" s="3">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K32" s="3">
-        <v>70000</v>
+        <v>5000</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="M32" s="3">
-        <v>1008</v>
+        <v>0</v>
       </c>
       <c r="N32" s="3">
-        <v>96200.031149999995</v>
+        <v>13996.97243</v>
       </c>
       <c r="O32" s="3">
-        <v>1.37429</v>
+        <v>2.7993899999999998</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>16</v>
+        <v>199</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>110</v>
+        <v>162</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="H33" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K33" s="3">
-        <v>30000</v>
+        <v>5000</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="M33" s="3">
-        <v>520000</v>
+        <v>0</v>
       </c>
       <c r="N33" s="3">
-        <v>39.928170000000001</v>
+        <v>2245.7130099999999</v>
       </c>
       <c r="O33" s="3">
-        <v>1.33E-3</v>
+        <v>0.44913999999999998</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>213</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E34" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="F34" s="4" t="s">
-        <v>110</v>
-      </c>
       <c r="G34" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="H34" s="3">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K34" s="3">
-        <v>10000</v>
+        <v>70000</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M34" s="3">
-        <v>5105000</v>
+        <v>832</v>
       </c>
       <c r="N34" s="3">
-        <v>15.14242</v>
+        <v>91430.407670000001</v>
       </c>
       <c r="O34" s="3">
-        <v>1.5100000000000001E-3</v>
+        <v>1.3061499999999999</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>219</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>225</v>
+        <v>116</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H35" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K35" s="3">
-        <v>15000</v>
+        <v>10000</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="M35" s="3">
-        <v>4808</v>
+        <v>4245000</v>
       </c>
       <c r="N35" s="3">
-        <v>3475.06576</v>
+        <v>14.44214</v>
       </c>
       <c r="O35" s="3">
-        <v>0.23166999999999999</v>
+        <v>1.4400000000000001E-3</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>16</v>
+        <v>225</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>16</v>
+        <v>226</v>
       </c>
       <c r="H36" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K36" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="K36" s="3">
+        <v>15000</v>
+      </c>
       <c r="L36" s="4" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="M36" s="3">
-        <v>0</v>
-      </c>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
+        <v>16558</v>
+      </c>
+      <c r="N36" s="3">
+        <v>3302.8062</v>
+      </c>
+      <c r="O36" s="3">
+        <v>0.22019</v>
+      </c>
       <c r="P36" s="2" t="s">
-        <v>16</v>
+        <v>228</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>32</v>
+        <v>229</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>236</v>
+        <v>215</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>238</v>
+        <v>20</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>237</v>
+        <v>20</v>
       </c>
       <c r="H37" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K37" s="3">
-        <v>5000</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="K37" s="3"/>
       <c r="L37" s="4" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="M37" s="3">
-        <v>37511</v>
-      </c>
-      <c r="N37" s="3">
-        <v>30.244990000000001</v>
-      </c>
-      <c r="O37" s="3">
-        <v>6.0499999999999998E-3</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
       <c r="P37" s="2" t="s">
-        <v>240</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>236</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>238</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="H38" s="3">
         <v>1</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K38" s="3">
         <v>5000</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="M38" s="3">
-        <v>1339</v>
+        <v>56013</v>
       </c>
       <c r="N38" s="3">
-        <v>30.244990000000001</v>
+        <v>28.725570000000001</v>
       </c>
       <c r="O38" s="3">
-        <v>6.0499999999999998E-3</v>
+        <v>5.7499999999999999E-3</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>246</v>
+        <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>110</v>
+        <v>238</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="H39" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K39" s="3">
-        <v>20000</v>
+        <v>5000</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="M39" s="3">
-        <v>273551</v>
+        <v>8</v>
       </c>
       <c r="N39" s="3">
-        <v>75.233919999999998</v>
+        <v>28.725570000000001</v>
       </c>
       <c r="O39" s="3">
-        <v>3.7599999999999999E-3</v>
+        <v>5.7499999999999999E-3</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -3370,853 +3371,959 @@
         <v>246</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>249</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="H40" s="3">
         <v>4</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K40" s="3">
         <v>20000</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="M40" s="3">
-        <v>7123408</v>
+        <v>472049</v>
       </c>
       <c r="N40" s="3">
-        <v>75.233919999999998</v>
+        <v>71.575879999999998</v>
       </c>
       <c r="O40" s="3">
-        <v>3.7599999999999999E-3</v>
+        <v>3.5799999999999998E-3</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>264</v>
+        <v>116</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="H41" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K41" s="3">
-        <v>5000</v>
+        <v>20000</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="M41" s="3">
-        <v>4130</v>
+        <v>6559357</v>
       </c>
       <c r="N41" s="3">
-        <v>1039.08878</v>
+        <v>71.575879999999998</v>
       </c>
       <c r="O41" s="3">
-        <v>0.20782</v>
+        <v>3.5799999999999998E-3</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>16</v>
+        <v>259</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>219</v>
+        <v>260</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>216</v>
+        <v>260</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>232</v>
+        <v>263</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>110</v>
+        <v>264</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="H42" s="3">
         <v>1</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K42" s="3">
         <v>5000</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="M42" s="3">
-        <v>15896421</v>
+        <v>84</v>
       </c>
       <c r="N42" s="3">
-        <v>10.599690000000001</v>
+        <v>5568.3176400000002</v>
       </c>
       <c r="O42" s="3">
-        <v>2.1199999999999999E-3</v>
+        <v>1.1136600000000001</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>271</v>
+        <v>219</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>232</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>274</v>
+        <v>116</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="H43" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K43" s="3">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="M43" s="3">
-        <v>755822</v>
+        <v>12929409</v>
       </c>
       <c r="N43" s="3">
-        <v>10.28091</v>
+        <v>20.15551</v>
       </c>
       <c r="O43" s="3">
-        <v>2.0600000000000002E-3</v>
+        <v>2.0200000000000001E-3</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>271</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>213</v>
+        <v>271</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>232</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>110</v>
+        <v>274</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="H44" s="3">
         <v>1</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K44" s="3">
         <v>5000</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="M44" s="3">
-        <v>732429</v>
+        <v>285314</v>
       </c>
       <c r="N44" s="3">
-        <v>10.599690000000001</v>
+        <v>9.80002</v>
       </c>
       <c r="O44" s="3">
-        <v>2.1199999999999999E-3</v>
+        <v>1.9599999999999999E-3</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>16</v>
+        <v>271</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>16</v>
+        <v>278</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>281</v>
+        <v>215</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>283</v>
+        <v>116</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="H45" s="3">
         <v>1</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K45" s="3">
         <v>5000</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="M45" s="3">
-        <v>10000</v>
+        <v>642324</v>
       </c>
       <c r="N45" s="3">
-        <v>14004.227730000001</v>
+        <v>10.07776</v>
       </c>
       <c r="O45" s="3">
-        <v>2.8008500000000001</v>
+        <v>2.0200000000000001E-3</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F46" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C46" s="2" t="s">
+      <c r="G46" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="H46" s="3">
+        <v>2</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K46" s="3">
+        <v>15000</v>
+      </c>
+      <c r="L46" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="H46" s="3">
-        <v>1</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K46" s="3">
-        <v>5000</v>
-      </c>
-      <c r="L46" s="4" t="s">
-        <v>290</v>
-      </c>
       <c r="M46" s="3">
-        <v>0</v>
+        <v>6480000</v>
       </c>
       <c r="N46" s="3">
-        <v>14027.419540000001</v>
+        <v>41.183900000000001</v>
       </c>
       <c r="O46" s="3">
-        <v>2.8054800000000002</v>
+        <v>2.7499999999999998E-3</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="G47" s="4" t="s">
         <v>292</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>296</v>
       </c>
       <c r="H47" s="3">
         <v>1</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K47" s="3">
         <v>5000</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="M47" s="3">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="N47" s="3">
-        <v>48000</v>
+        <v>13309.85987</v>
       </c>
       <c r="O47" s="3">
-        <v>9.6</v>
+        <v>2.6619700000000002</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="H48" s="3">
+        <v>1</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K48" s="3">
+        <v>5000</v>
+      </c>
+      <c r="L48" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="H48" s="3">
-        <v>3</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K48" s="3">
-        <v>15000</v>
-      </c>
-      <c r="L48" s="4" t="s">
-        <v>302</v>
-      </c>
       <c r="M48" s="3">
-        <v>5594</v>
+        <v>0</v>
       </c>
       <c r="N48" s="3">
-        <v>59551.550130000003</v>
+        <v>13331.91984</v>
       </c>
       <c r="O48" s="3">
-        <v>3.9701</v>
+        <v>2.6663800000000002</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="F49" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="C49" s="2" t="s">
+      <c r="G49" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>307</v>
       </c>
       <c r="H49" s="3">
         <v>1</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K49" s="3">
         <v>5000</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="M49" s="3">
         <v>0</v>
       </c>
       <c r="N49" s="3">
-        <v>14496.555609999999</v>
+        <v>48000</v>
       </c>
       <c r="O49" s="3">
-        <v>2.8993099999999998</v>
+        <v>9.6</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="G50" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C50" s="2" t="s">
+      <c r="H50" s="3">
+        <v>3</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K50" s="3">
+        <v>15000</v>
+      </c>
+      <c r="L50" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="H50" s="3">
-        <v>1</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="K50" s="3"/>
-      <c r="L50" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="M50" s="3"/>
-      <c r="N50" s="3"/>
-      <c r="O50" s="3"/>
+      <c r="M50" s="3">
+        <v>5438</v>
+      </c>
+      <c r="N50" s="3">
+        <v>56599.061999999998</v>
+      </c>
+      <c r="O50" s="3">
+        <v>3.7732700000000001</v>
+      </c>
       <c r="P50" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F51" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="G51" s="4" t="s">
         <v>315</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>317</v>
       </c>
       <c r="H51" s="3">
         <v>1</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K51" s="3">
         <v>5000</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="M51" s="3">
         <v>0</v>
       </c>
       <c r="N51" s="3">
-        <v>1570.5478599999999</v>
+        <v>13777.80106</v>
       </c>
       <c r="O51" s="3">
-        <v>0.31411</v>
+        <v>2.75556</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="F52" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="D52" s="2" t="s">
+      <c r="G52" s="4" t="s">
         <v>319</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>322</v>
       </c>
       <c r="H52" s="3">
         <v>1</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>30</v>
+        <v>320</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K52" s="3">
-        <v>5000</v>
-      </c>
+        <v>319</v>
+      </c>
+      <c r="K52" s="3"/>
       <c r="L52" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="M52" s="3">
-        <v>976</v>
-      </c>
-      <c r="N52" s="3">
-        <v>11050.37998</v>
-      </c>
-      <c r="O52" s="3">
-        <v>2.21008</v>
-      </c>
+        <v>321</v>
+      </c>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
       <c r="P52" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="D53" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="G53" s="4" t="s">
         <v>325</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>330</v>
       </c>
       <c r="H53" s="3">
         <v>1</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K53" s="3">
         <v>5000</v>
       </c>
       <c r="L53" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="M53" s="3">
+        <v>3000</v>
+      </c>
+      <c r="N53" s="3">
+        <v>1492.6982700000001</v>
+      </c>
+      <c r="O53" s="3">
+        <v>0.29854000000000003</v>
+      </c>
+      <c r="P53" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="H54" s="3">
+        <v>1</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K54" s="3">
+        <v>5000</v>
+      </c>
+      <c r="L54" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="M53" s="3">
+      <c r="M54" s="3">
+        <v>899</v>
+      </c>
+      <c r="N54" s="3">
+        <v>10502.292079999999</v>
+      </c>
+      <c r="O54" s="3">
+        <v>2.10046</v>
+      </c>
+      <c r="P54" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="H55" s="3">
+        <v>1</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K55" s="3">
+        <v>5000</v>
+      </c>
+      <c r="L55" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="M55" s="3">
         <v>0</v>
       </c>
-      <c r="N53" s="3">
-        <v>4978.0704599999999</v>
-      </c>
-      <c r="O53" s="3">
-        <v>0.99560999999999999</v>
-      </c>
-      <c r="P53" s="2" t="s">
-        <v>16</v>
+      <c r="N55" s="3">
+        <v>4731.2290199999998</v>
+      </c>
+      <c r="O55" s="3">
+        <v>0.94625000000000004</v>
+      </c>
+      <c r="P55" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" tooltip="Component" display="'LINEAR TECHNOLOGY"/>
-    <hyperlink ref="G2" tooltip="Manufacturer" display="'LTC7103IUHE#PBF"/>
-    <hyperlink ref="L2" tooltip="Supplier" display="'24AC4318"/>
-    <hyperlink ref="F3" tooltip="Component" display="'Hirose Electric Co Ltd"/>
-    <hyperlink ref="G3" tooltip="Manufacturer" display="'DF40C(2.0)-30DS-0.4V(51)"/>
-    <hyperlink ref="L3" tooltip="Supplier" display="'H11771TR-ND"/>
-    <hyperlink ref="F4" tooltip="Component" display="'"/>
-    <hyperlink ref="G4" tooltip="Manufacturer" display="'"/>
-    <hyperlink ref="L4" tooltip="Supplier" display="'GRM188R71C102KA01D-ND"/>
-    <hyperlink ref="F5" tooltip="Component" display="'Murata Electronics North America"/>
-    <hyperlink ref="G5" tooltip="Manufacturer" display="'GRM155R62A104KE14D"/>
-    <hyperlink ref="L5" tooltip="Supplier" display="'490-10458-2-ND"/>
-    <hyperlink ref="F6" tooltip="Component" display="'TDK Corporation"/>
-    <hyperlink ref="G6" tooltip="Manufacturer" display="'C3216X5R1A107M160AC"/>
-    <hyperlink ref="L6" tooltip="Supplier" display="'445-6007-2-ND"/>
-    <hyperlink ref="F7" tooltip="Component" display="'AVX Corporation"/>
-    <hyperlink ref="G7" tooltip="Manufacturer" display="'0603YC104JAT2A"/>
-    <hyperlink ref="L7" tooltip="Supplier" display="'478-3726-1-ND"/>
-    <hyperlink ref="F8" tooltip="Component" display="'TDK Corporation"/>
-    <hyperlink ref="G8" tooltip="Manufacturer" display="'C3216X7S1A226M160AC"/>
-    <hyperlink ref="L8" tooltip="Supplier" display="'445-8035-1-ND"/>
-    <hyperlink ref="F9" tooltip="Component" display="'Taiyo Yuden"/>
-    <hyperlink ref="G9" tooltip="Manufacturer" display="'HMK325B7225KN-T"/>
-    <hyperlink ref="L9" tooltip="Supplier" display="'587-1778-1-ND"/>
-    <hyperlink ref="F10" tooltip="Component" display="'Murata Electronics North America"/>
-    <hyperlink ref="G10" tooltip="Manufacturer" display="'GRM188R70J105KA01D"/>
-    <hyperlink ref="L10" tooltip="Supplier" display="'490-3898-1-ND"/>
-    <hyperlink ref="F11" tooltip="Component" display="'TDK Corporation"/>
-    <hyperlink ref="G11" tooltip="Manufacturer" display="'C1608X7S2A473K080AB"/>
-    <hyperlink ref="L11" tooltip="Supplier" display="'445-6032-1-ND"/>
-    <hyperlink ref="F12" tooltip="Component" display="'Murata Electronics North America"/>
-    <hyperlink ref="G12" tooltip="Manufacturer" display="'GRM21BC72A105KE01L"/>
-    <hyperlink ref="L12" tooltip="Supplier" display="'490-14464-2-ND"/>
-    <hyperlink ref="F13" tooltip="Component" display="'Murata Electronics North America"/>
-    <hyperlink ref="G13" tooltip="Manufacturer" display="'GRM32ER71K475KE14L"/>
-    <hyperlink ref="L13" tooltip="Supplier" display="'490-9972-1-ND"/>
-    <hyperlink ref="F14" tooltip="Component" display="'TDK Corporation"/>
-    <hyperlink ref="G14" tooltip="Manufacturer" display="'CGA2B3X7R1H103K050BB"/>
-    <hyperlink ref="L14" tooltip="Supplier" display="'445-6893-1-ND"/>
-    <hyperlink ref="F15" tooltip="Component" display="'TDK Corporation"/>
-    <hyperlink ref="G15" tooltip="Manufacturer" display="'C1608X6S1C225K080AC"/>
-    <hyperlink ref="L15" tooltip="Supplier" display="'445-7438-1-ND"/>
-    <hyperlink ref="F16" tooltip="Component" display="'Yageo"/>
-    <hyperlink ref="G16" tooltip="Manufacturer" display="'CC0402ZRY5V7BB104"/>
-    <hyperlink ref="L16" tooltip="Supplier" display="'311-1047-1-ND"/>
-    <hyperlink ref="F17" tooltip="Component" display="'Murata Electronics North America"/>
-    <hyperlink ref="G17" tooltip="Manufacturer" display="'GRM033C81E104ME14D"/>
-    <hyperlink ref="L17" tooltip="Supplier" display="'490-10404-2-ND"/>
-    <hyperlink ref="F18" tooltip="Component" display="'TDK"/>
-    <hyperlink ref="G18" tooltip="Manufacturer" display="'CGA9P3X7S2A156M250KB"/>
-    <hyperlink ref="L18" tooltip="Supplier" display="'80X3236"/>
-    <hyperlink ref="F19" tooltip="Component" display="'Murata Electronics North America"/>
-    <hyperlink ref="G19" tooltip="Manufacturer" display="'GRM0335C1H8R0DA01J"/>
-    <hyperlink ref="L19" tooltip="Supplier" display="'490-13331-1-ND"/>
-    <hyperlink ref="F20" tooltip="Component" display="'Murata Electronics North America"/>
-    <hyperlink ref="G20" tooltip="Manufacturer" display="'GRM21BR60G107ME15L"/>
-    <hyperlink ref="L20" tooltip="Supplier" display="'490-10510-1-ND"/>
-    <hyperlink ref="F21" tooltip="Component" display="'Murata Electronics North America"/>
-    <hyperlink ref="G21" tooltip="Manufacturer" display="'GRM033R60J225ME15D"/>
-    <hyperlink ref="L21" tooltip="Supplier" display="'490-13224-1-ND"/>
-    <hyperlink ref="F22" tooltip="Component" display="'AVX Corporation"/>
-    <hyperlink ref="G22" tooltip="Manufacturer" display="'04026D226MAT2A"/>
-    <hyperlink ref="L22" tooltip="Supplier" display="'478-9839-2-ND"/>
-    <hyperlink ref="F23" tooltip="Component" display="'Murata Electronics North America"/>
-    <hyperlink ref="G23" tooltip="Manufacturer" display="'GRM035R60J475ME15D"/>
-    <hyperlink ref="L23" tooltip="Supplier" display="'490-13230-2-ND"/>
-    <hyperlink ref="F24" tooltip="Component" display="'Murata Electronics North America"/>
-    <hyperlink ref="G24" tooltip="Manufacturer" display="'GRM033R60J105MEA2D"/>
-    <hyperlink ref="L24" tooltip="Supplier" display="'490-7229-2-ND"/>
-    <hyperlink ref="F25" tooltip="Component" display="'JST Sales America Inc."/>
-    <hyperlink ref="G25" tooltip="Manufacturer" display="'BM04B-GHS-TBT(LF)(SN)(N)"/>
-    <hyperlink ref="L25" tooltip="Supplier" display="'455-1580-2-ND"/>
-    <hyperlink ref="F26" tooltip="Component" display="'ON Semiconductor"/>
-    <hyperlink ref="G26" tooltip="Manufacturer" display="'MBR1H100SFT3G"/>
-    <hyperlink ref="L26" tooltip="Supplier" display="'MBR1H100SFT3GOSCT-ND"/>
-    <hyperlink ref="F27" tooltip="Component" display="'ON Semiconductor"/>
-    <hyperlink ref="G27" tooltip="Manufacturer" display="'RB751V40T1G"/>
-    <hyperlink ref="L27" tooltip="Supplier" display="'RB751V40T1GOSCT-ND"/>
-    <hyperlink ref="F28" tooltip="Component" display="'Murata Electronics North America"/>
-    <hyperlink ref="G28" tooltip="Manufacturer" display="'NFM18PC225B1A3D"/>
-    <hyperlink ref="L28" tooltip="Supplier" display="'490-6972-1-ND"/>
-    <hyperlink ref="F29" tooltip="Component" display="'Eaton"/>
-    <hyperlink ref="G29" tooltip="Manufacturer" display="'SD53-150-R"/>
-    <hyperlink ref="L29" tooltip="Supplier" display="'513-1458-1-ND"/>
-    <hyperlink ref="F30" tooltip="Component" display="'Wurth Electronics Inc."/>
-    <hyperlink ref="G30" tooltip="Manufacturer" display="'7443551181"/>
-    <hyperlink ref="L30" tooltip="Supplier" display="'732-3880-2-ND"/>
-    <hyperlink ref="F31" tooltip="Component" display="'JST Sales America Inc."/>
-    <hyperlink ref="G31" tooltip="Manufacturer" display="'SM06B-SURS-TF(LF)(SN)"/>
-    <hyperlink ref="L31" tooltip="Supplier" display="'SM06B-SURS-TF(LF)(SN)-ND"/>
-    <hyperlink ref="F32" tooltip="Component" display="'Texas Instruments"/>
-    <hyperlink ref="G32" tooltip="Manufacturer" display="'CSD19502Q5B"/>
-    <hyperlink ref="L32" tooltip="Supplier" display="'296-37194-1-ND"/>
-    <hyperlink ref="F33" tooltip="Component" display="'Yageo"/>
-    <hyperlink ref="G33" tooltip="Manufacturer" display="'RC0402JR-07120RL"/>
-    <hyperlink ref="L33" tooltip="Supplier" display="'311-120JRTR-ND"/>
-    <hyperlink ref="F34" tooltip="Component" display="'Yageo"/>
-    <hyperlink ref="G34" tooltip="Manufacturer" display="'RC0402JR-0710KL"/>
-    <hyperlink ref="L34" tooltip="Supplier" display="'311-10KJRTR-ND"/>
-    <hyperlink ref="F35" tooltip="Component" display="'Stackpole Electronics Inc."/>
-    <hyperlink ref="G35" tooltip="Manufacturer" display="'CSNL2010FT1L00"/>
-    <hyperlink ref="L35" tooltip="Supplier" display="'CSNL2010FT1L00CT-ND"/>
-    <hyperlink ref="F36" r:id="rId1" tooltip="Component" display="'"/>
-    <hyperlink ref="G36" r:id="rId2" tooltip="Manufacturer" display="'"/>
-    <hyperlink ref="L36" r:id="rId3" tooltip="Supplier" display="'311-2.0KLRCT-ND"/>
-    <hyperlink ref="F37" tooltip="Component" display="'Vishay Dale"/>
-    <hyperlink ref="G37" tooltip="Manufacturer" display="'CRCW060328K0FKEA"/>
-    <hyperlink ref="L37" tooltip="Supplier" display="'541-28.0KHCT-ND"/>
-    <hyperlink ref="F38" tooltip="Component" display="'Vishay Dale"/>
-    <hyperlink ref="G38" tooltip="Manufacturer" display="'CRCW06038K45FKEA"/>
-    <hyperlink ref="L38" tooltip="Supplier" display="'541-8.45KHCT-ND"/>
-    <hyperlink ref="F39" tooltip="Component" display="'Yageo"/>
-    <hyperlink ref="G39" tooltip="Manufacturer" display="'RC0805FR-0718KL"/>
-    <hyperlink ref="L39" tooltip="Supplier" display="'311-18.0KCRCT-ND"/>
-    <hyperlink ref="F40" tooltip="Component" display="'Yageo"/>
-    <hyperlink ref="G40" tooltip="Manufacturer" display="'RC0805FR-071KL"/>
-    <hyperlink ref="L40" tooltip="Supplier" display="'311-1.00KCRCT-ND"/>
-    <hyperlink ref="F41" tooltip="Component" display="'TE Connectivity Passive Product"/>
-    <hyperlink ref="G41" tooltip="Manufacturer" display="'35221R2JT"/>
-    <hyperlink ref="L41" tooltip="Supplier" display="'A121178CT-ND"/>
-    <hyperlink ref="F42" tooltip="Component" display="'Yageo"/>
-    <hyperlink ref="G42" tooltip="Manufacturer" display="'RC0402FR-0710KL"/>
-    <hyperlink ref="L42" tooltip="Supplier" display="'311-10.0KLRCT-ND"/>
-    <hyperlink ref="F43" tooltip="Component" display="'Samsung Electro-Mechanics America, Inc."/>
-    <hyperlink ref="G43" tooltip="Manufacturer" display="'RC1005F102CS"/>
-    <hyperlink ref="L43" tooltip="Supplier" display="'1276-3430-1-ND"/>
-    <hyperlink ref="F44" tooltip="Component" display="'Yageo"/>
-    <hyperlink ref="G44" tooltip="Manufacturer" display="'RC0402FR-07120RL"/>
-    <hyperlink ref="L44" tooltip="Supplier" display="'311-120LRCT-ND"/>
-    <hyperlink ref="F45" tooltip="Component" display="'STMicroelectronics"/>
-    <hyperlink ref="G45" tooltip="Manufacturer" display="'VL53L0CXV0DH/1"/>
-    <hyperlink ref="L45" tooltip="Supplier" display="'497-16538-2-ND"/>
-    <hyperlink ref="F46" tooltip="Component" display="'Texas Instruments"/>
-    <hyperlink ref="G46" tooltip="Manufacturer" display="'DRV8323RHRGZR"/>
-    <hyperlink ref="L46" tooltip="Supplier" display="'DRV8323RHRGZR-ND"/>
-    <hyperlink ref="F47" tooltip="Component" display="'STMICROELECTRONICS"/>
-    <hyperlink ref="G47" tooltip="Manufacturer" display="'STM32F769AIY6TR"/>
-    <hyperlink ref="L47" tooltip="Supplier" display="'84Y8745"/>
-    <hyperlink ref="F48" tooltip="Component" display="'NXP USA Inc."/>
-    <hyperlink ref="G48" tooltip="Manufacturer" display="'TJA1052IT/5Y"/>
-    <hyperlink ref="L48" tooltip="Supplier" display="'568-11942-1-ND"/>
-    <hyperlink ref="F49" tooltip="Component" display="'Monolithic Power Systems Inc."/>
-    <hyperlink ref="G49" tooltip="Manufacturer" display="'MA700GQ-Z"/>
-    <hyperlink ref="L49" tooltip="Supplier" display="'MA700GQ-Z-ND"/>
-    <hyperlink ref="F50" tooltip="Component" display="'Supplier disabled"/>
-    <hyperlink ref="G50" tooltip="Manufacturer" display="'Supplier disabled"/>
-    <hyperlink ref="L50" tooltip="Supplier" display="'Component Distributors Inc. - ICM-20649"/>
-    <hyperlink ref="F51" tooltip="Component" display="'ON Semiconductor"/>
-    <hyperlink ref="G51" tooltip="Manufacturer" display="'NCV8154MTW180280TCG"/>
-    <hyperlink ref="L51" tooltip="Supplier" display="'NCV8154MTW180280TCGOSTR-ND"/>
-    <hyperlink ref="F52" tooltip="Component" display="'Linear Technology"/>
-    <hyperlink ref="G52" tooltip="Manufacturer" display="'LTC4316IDD#PBF"/>
-    <hyperlink ref="L52" tooltip="Supplier" display="'LTC4316IDD#PBF-ND"/>
-    <hyperlink ref="F53" tooltip="Component" display="'TXC CORPORATION"/>
-    <hyperlink ref="G53" tooltip="Manufacturer" display="'8Q-24.000MEEV-T"/>
-    <hyperlink ref="L53" tooltip="Supplier" display="'887-1846-2-ND"/>
+    <hyperlink ref="F2" tooltip="Component" display="'" xr:uid="{B31F896F-2527-4816-9332-071E762B1215}"/>
+    <hyperlink ref="G2" tooltip="Manufacturer" display="'" xr:uid="{9BA091F0-D52F-4CA1-9982-6DC1CD901A1A}"/>
+    <hyperlink ref="L2" tooltip="Supplier" display="'" xr:uid="{F507E53B-2D49-47B9-96E6-AA29E1DA3DA9}"/>
+    <hyperlink ref="F3" tooltip="Component" display="'LINEAR TECHNOLOGY" xr:uid="{5EE8532A-AF60-4E20-9BC6-0C7B8AA9084E}"/>
+    <hyperlink ref="G3" tooltip="Manufacturer" display="'LTC7103IUHE#PBF" xr:uid="{9CEAA963-4FF5-4EEB-9242-A7773A4C316F}"/>
+    <hyperlink ref="L3" tooltip="Supplier" display="'24AC4318" xr:uid="{93B4927C-F750-470E-BD16-6B6AD68D81C0}"/>
+    <hyperlink ref="F4" tooltip="Component" display="'" xr:uid="{F53A0377-465E-4708-9943-7B7E360F3629}"/>
+    <hyperlink ref="G4" tooltip="Manufacturer" display="'" xr:uid="{06118D1D-69D6-47C4-B624-0420819616C9}"/>
+    <hyperlink ref="L4" tooltip="Supplier" display="'" xr:uid="{CCC4F0B8-AC91-40D6-A461-B1FCC0DA379B}"/>
+    <hyperlink ref="F5" tooltip="Component" display="'Hirose Electric Co Ltd" xr:uid="{DB8F3FF0-3092-40CE-979F-FA6D8662E3F9}"/>
+    <hyperlink ref="G5" tooltip="Manufacturer" display="'DF40C(2.0)-30DS-0.4V(51)" xr:uid="{13623740-F959-4A07-B4F2-0A60058B3F41}"/>
+    <hyperlink ref="L5" tooltip="Supplier" display="'H11771TR-ND" xr:uid="{809D2833-AEF1-47D9-A985-64D0BBAA08DD}"/>
+    <hyperlink ref="F6" tooltip="Component" display="'" xr:uid="{54251C50-044A-4D93-B209-93737173D631}"/>
+    <hyperlink ref="G6" tooltip="Manufacturer" display="'" xr:uid="{44D5DCBA-88BE-4D3A-8601-567CAE71F553}"/>
+    <hyperlink ref="L6" tooltip="Supplier" display="'GRM188R71C102KA01D-ND" xr:uid="{8C25ECC1-2C38-41A4-8692-F98D1CAA157C}"/>
+    <hyperlink ref="F7" tooltip="Component" display="'Murata Electronics North America" xr:uid="{174EDD3C-D2A3-4603-BF2A-29C147F03B84}"/>
+    <hyperlink ref="G7" tooltip="Manufacturer" display="'GRM155R62A104KE14D" xr:uid="{7E2F0AF2-2F4F-4C53-8D83-91D2B44C565A}"/>
+    <hyperlink ref="L7" tooltip="Supplier" display="'490-10458-2-ND" xr:uid="{78E464E6-3EB9-4ADD-8437-6B18B7C5A950}"/>
+    <hyperlink ref="F8" tooltip="Component" display="'TDK Corporation" xr:uid="{9C3964A3-5C35-4BCD-802B-AA9743415471}"/>
+    <hyperlink ref="G8" tooltip="Manufacturer" display="'C3216X5R1A107M160AC" xr:uid="{84C5F065-6C92-4932-8A6A-799EAA7D0B6B}"/>
+    <hyperlink ref="L8" tooltip="Supplier" display="'445-6007-2-ND" xr:uid="{C0E9065E-224E-4CDD-A066-B2C2C57DD668}"/>
+    <hyperlink ref="F9" tooltip="Component" display="'AVX Corporation" xr:uid="{0B6AA0FA-458E-445B-B774-74E51CDAA983}"/>
+    <hyperlink ref="G9" tooltip="Manufacturer" display="'0603YC104JAT2A" xr:uid="{20BA1E25-23FC-4564-BA32-CDFC3A97B91F}"/>
+    <hyperlink ref="L9" tooltip="Supplier" display="'478-3726-1-ND" xr:uid="{6CE1C924-818B-4477-9FF4-AD7474506203}"/>
+    <hyperlink ref="F10" tooltip="Component" display="'TDK Corporation" xr:uid="{0C8C3DAC-115C-4455-9AC7-F79E82D4A4B6}"/>
+    <hyperlink ref="G10" tooltip="Manufacturer" display="'C3216X7S1A226M160AC" xr:uid="{393E6E3C-6F13-4C4A-8A06-C1386610EA24}"/>
+    <hyperlink ref="L10" tooltip="Supplier" display="'445-8035-1-ND" xr:uid="{DE700F91-73F4-4DEB-B737-67F63612DBC3}"/>
+    <hyperlink ref="F11" tooltip="Component" display="'Taiyo Yuden" xr:uid="{F886E223-2781-4EF7-9BD1-35780C02AE69}"/>
+    <hyperlink ref="G11" tooltip="Manufacturer" display="'HMK325B7225KN-T" xr:uid="{CD68346D-9639-4A55-848B-CD91199037D9}"/>
+    <hyperlink ref="L11" tooltip="Supplier" display="'587-1778-1-ND" xr:uid="{4DD6DA28-AD4C-40B7-B32B-F66BAE8BBDE3}"/>
+    <hyperlink ref="F12" tooltip="Component" display="'Murata Electronics North America" xr:uid="{5A3C6461-B026-4D64-B817-87048DF135D7}"/>
+    <hyperlink ref="G12" tooltip="Manufacturer" display="'GRM188R70J105KA01D" xr:uid="{2D2C9A79-B0F1-45C7-8CB4-0C66574091C4}"/>
+    <hyperlink ref="L12" tooltip="Supplier" display="'490-3898-1-ND" xr:uid="{4510B9D2-AEE0-4F1F-8841-E55318DF83EA}"/>
+    <hyperlink ref="F13" tooltip="Component" display="'TDK Corporation" xr:uid="{129A9181-2381-4108-AA70-BBC35F94CA3B}"/>
+    <hyperlink ref="G13" tooltip="Manufacturer" display="'C1608X7S2A473K080AB" xr:uid="{A7D4ADD8-416B-470D-A02D-5795F1239C73}"/>
+    <hyperlink ref="L13" tooltip="Supplier" display="'445-6032-1-ND" xr:uid="{3B4B68A9-260F-4FC0-8A3D-949BC47BD408}"/>
+    <hyperlink ref="F14" tooltip="Component" display="'Murata Electronics North America" xr:uid="{6448E8DF-6081-4841-A438-9B99EC35D780}"/>
+    <hyperlink ref="G14" tooltip="Manufacturer" display="'GRM21BC72A105KE01L" xr:uid="{7CC4E3E5-F2A6-4BFD-B5EC-5957FC5D402F}"/>
+    <hyperlink ref="L14" tooltip="Supplier" display="'490-14464-2-ND" xr:uid="{39B37AA2-367B-418C-B555-F37B1108E524}"/>
+    <hyperlink ref="F15" tooltip="Component" display="'Murata Electronics North America" xr:uid="{660E911B-7C77-45D6-91DB-782E98D18D0D}"/>
+    <hyperlink ref="G15" tooltip="Manufacturer" display="'GRM32ER71K475KE14L" xr:uid="{015B19D1-9616-41A3-A369-6600DF12291C}"/>
+    <hyperlink ref="L15" tooltip="Supplier" display="'490-9972-1-ND" xr:uid="{167B686F-5133-4D90-9B0C-8BCEE7605547}"/>
+    <hyperlink ref="F16" tooltip="Component" display="'TDK Corporation" xr:uid="{AA55DE7D-DB0F-455E-A553-8883A2EE3422}"/>
+    <hyperlink ref="G16" tooltip="Manufacturer" display="'CGA2B3X7R1H103K050BB" xr:uid="{51A7AB96-95B2-4C6B-851E-04200F8D9DC8}"/>
+    <hyperlink ref="L16" tooltip="Supplier" display="'445-6893-1-ND" xr:uid="{77036401-E2EF-4A20-B97B-355F6E4AA4A2}"/>
+    <hyperlink ref="F17" tooltip="Component" display="'TDK Corporation" xr:uid="{FB30B0BA-7C68-48AF-BC98-1F5F420F1809}"/>
+    <hyperlink ref="G17" tooltip="Manufacturer" display="'C1608X6S1C225K080AC" xr:uid="{E9E65E3B-143E-42A6-8D23-FC51AFCA6BDF}"/>
+    <hyperlink ref="L17" tooltip="Supplier" display="'445-7438-1-ND" xr:uid="{C6D74A51-341D-4080-ABA1-14EEE3592B7E}"/>
+    <hyperlink ref="F18" tooltip="Component" display="'Yageo" xr:uid="{91D233BE-A721-46B4-A4AD-999E42FC6D15}"/>
+    <hyperlink ref="G18" tooltip="Manufacturer" display="'CC0402ZRY5V7BB104" xr:uid="{997B8282-9477-46A3-84A2-57BB9382FFCB}"/>
+    <hyperlink ref="L18" tooltip="Supplier" display="'311-1047-1-ND" xr:uid="{BEB2B6B3-E87A-4A2D-9E63-CAB59E91BDE6}"/>
+    <hyperlink ref="F19" tooltip="Component" display="'Murata Electronics North America" xr:uid="{0E0215AD-1ADD-439B-96BE-0AA8C7F8664F}"/>
+    <hyperlink ref="G19" tooltip="Manufacturer" display="'GRM033C81E104ME14D" xr:uid="{F03D4C10-4684-465C-9CC4-788CCB521396}"/>
+    <hyperlink ref="L19" tooltip="Supplier" display="'490-10404-2-ND" xr:uid="{631D98B4-6C36-48E1-A823-34F2595219A5}"/>
+    <hyperlink ref="F20" tooltip="Component" display="'TDK" xr:uid="{61F7CB01-728B-48CB-A8AA-E608C85AC2C7}"/>
+    <hyperlink ref="G20" tooltip="Manufacturer" display="'CGA9P3X7S2A156M250KB" xr:uid="{C41062F8-C4F1-4D61-BDCD-EB634092824F}"/>
+    <hyperlink ref="L20" tooltip="Supplier" display="'80X3236" xr:uid="{E1EB349C-9E55-4626-A3F1-5B20680F519D}"/>
+    <hyperlink ref="F21" tooltip="Component" display="'Murata Electronics North America" xr:uid="{B538D1F8-0AFF-4AC3-B0B2-E873097FA825}"/>
+    <hyperlink ref="G21" tooltip="Manufacturer" display="'GRM0335C1H8R0DA01J" xr:uid="{2E6074D3-79DC-4CD8-AEFF-704CA4E4ECAA}"/>
+    <hyperlink ref="L21" tooltip="Supplier" display="'490-13331-1-ND" xr:uid="{069AB2E4-58A6-4AC6-BF1F-4382A92DB110}"/>
+    <hyperlink ref="F22" tooltip="Component" display="'Murata Electronics North America" xr:uid="{A39F6BC1-526F-4085-AA5D-F1721517AAB4}"/>
+    <hyperlink ref="G22" tooltip="Manufacturer" display="'GRM21BR60G107ME15L" xr:uid="{B81A4117-602B-46E9-9343-7B3E665DF39E}"/>
+    <hyperlink ref="L22" tooltip="Supplier" display="'490-10510-1-ND" xr:uid="{98C25F8A-4007-472E-9045-AB446B0FFE51}"/>
+    <hyperlink ref="F23" tooltip="Component" display="'Murata Electronics North America" xr:uid="{FC253C08-79A6-4E86-AA3F-3754EA103D36}"/>
+    <hyperlink ref="G23" tooltip="Manufacturer" display="'GRM033R60J225ME15D" xr:uid="{A2BD6246-5A5A-4161-8EB0-69B4B80E87FA}"/>
+    <hyperlink ref="L23" tooltip="Supplier" display="'490-13224-1-ND" xr:uid="{54D9A380-C245-4A26-9277-944DF989565F}"/>
+    <hyperlink ref="F24" tooltip="Component" display="'AVX Corporation" xr:uid="{BE36F10A-5CFD-4D76-80BD-89D3350E7953}"/>
+    <hyperlink ref="G24" tooltip="Manufacturer" display="'04026D226MAT2A" xr:uid="{E37CE664-F75D-4FFD-ACF1-0879C5010C9C}"/>
+    <hyperlink ref="L24" tooltip="Supplier" display="'478-9839-2-ND" xr:uid="{1EA49EF1-657C-417A-AF94-5B59A41D4B12}"/>
+    <hyperlink ref="F25" tooltip="Component" display="'Murata Electronics North America" xr:uid="{70FC6189-D9E1-4E33-A845-CBB2B25470F2}"/>
+    <hyperlink ref="G25" tooltip="Manufacturer" display="'GRM035R60J475ME15D" xr:uid="{B28DDAD2-D1DF-498F-926D-1865D623BB2B}"/>
+    <hyperlink ref="L25" tooltip="Supplier" display="'490-13230-2-ND" xr:uid="{48C42A3E-5447-43B8-9C05-EDDB1B60F672}"/>
+    <hyperlink ref="F26" tooltip="Component" display="'Murata Electronics North America" xr:uid="{99E59680-2505-4751-8620-3784859AE982}"/>
+    <hyperlink ref="G26" tooltip="Manufacturer" display="'GRM033R60J105MEA2D" xr:uid="{9D9E56BE-B389-453D-870E-1FE6ABCBA552}"/>
+    <hyperlink ref="L26" tooltip="Supplier" display="'490-7229-2-ND" xr:uid="{AD94FFF9-E565-4D27-9BF8-076BB7383761}"/>
+    <hyperlink ref="F27" tooltip="Component" display="'JST Sales America Inc." xr:uid="{D116DAF6-5E1F-45F9-AEC2-20BC39318CF6}"/>
+    <hyperlink ref="G27" tooltip="Manufacturer" display="'BM04B-GHS-TBT(LF)(SN)(N)" xr:uid="{957CCB55-9810-4441-B267-0414DCBEDA8B}"/>
+    <hyperlink ref="L27" tooltip="Supplier" display="'455-1580-2-ND" xr:uid="{BC52DCE2-745D-4A4F-A072-2D530C500E29}"/>
+    <hyperlink ref="F28" tooltip="Component" display="'ON Semiconductor" xr:uid="{44DA57D2-2014-46DD-8B14-D7E00AEA6653}"/>
+    <hyperlink ref="G28" tooltip="Manufacturer" display="'MBR1H100SFT3G" xr:uid="{17EF49BA-06A2-465A-BDA8-D486E6CB033A}"/>
+    <hyperlink ref="L28" tooltip="Supplier" display="'MBR1H100SFT3GOSCT-ND" xr:uid="{75D53C8E-65EF-40A0-AB15-0D43CD463221}"/>
+    <hyperlink ref="F29" tooltip="Component" display="'ON Semiconductor" xr:uid="{62AC20A0-8F58-43F6-A1AE-0C01B1B3440C}"/>
+    <hyperlink ref="G29" tooltip="Manufacturer" display="'RB751V40T1G" xr:uid="{0FF6ACE6-9AB5-4EF0-A0E6-B74215BA9605}"/>
+    <hyperlink ref="L29" tooltip="Supplier" display="'RB751V40T1GOSCT-ND" xr:uid="{89A4E7E0-8A9D-4808-A109-558A63625D18}"/>
+    <hyperlink ref="F30" tooltip="Component" display="'Murata Electronics North America" xr:uid="{6A42FC9B-9221-448B-B850-8392DC44079F}"/>
+    <hyperlink ref="G30" tooltip="Manufacturer" display="'NFM18PC225B1A3D" xr:uid="{F8BAA340-4A3C-4FBC-971B-135AF1B65694}"/>
+    <hyperlink ref="L30" tooltip="Supplier" display="'490-6972-1-ND" xr:uid="{B9DBBDB3-4709-4656-8AD0-D0EB0AE0C9AF}"/>
+    <hyperlink ref="F31" tooltip="Component" display="'Eaton" xr:uid="{51A40406-61F1-460A-947F-FE2CA6544C5C}"/>
+    <hyperlink ref="G31" tooltip="Manufacturer" display="'SD53-150-R" xr:uid="{B724BBF1-6DEE-499E-A4CB-FB1DB3695E6B}"/>
+    <hyperlink ref="L31" tooltip="Supplier" display="'513-1458-1-ND" xr:uid="{4B186DDB-FFF6-4E39-A190-D6664F1E3A13}"/>
+    <hyperlink ref="F32" tooltip="Component" display="'Wurth Electronics Inc." xr:uid="{0B4AA338-C425-4734-BAE3-BB6649F7044E}"/>
+    <hyperlink ref="G32" tooltip="Manufacturer" display="'7443551181" xr:uid="{2B584943-8A6D-48A7-B33B-5D138385277F}"/>
+    <hyperlink ref="L32" tooltip="Supplier" display="'732-3880-2-ND" xr:uid="{259FF567-4A64-48FD-B2FB-24CD6EFFFE75}"/>
+    <hyperlink ref="F33" tooltip="Component" display="'JST Sales America Inc." xr:uid="{7527C244-DE1E-4FAF-AC3B-5195251C9F53}"/>
+    <hyperlink ref="G33" tooltip="Manufacturer" display="'SM06B-SURS-TF(LF)(SN)" xr:uid="{9F26F367-19E7-49D9-84BE-8095BE647FBE}"/>
+    <hyperlink ref="L33" tooltip="Supplier" display="'SM06B-SURS-TF(LF)(SN)-ND" xr:uid="{738B557D-A415-4AE4-8767-C247BCEC3E10}"/>
+    <hyperlink ref="F34" tooltip="Component" display="'Texas Instruments" xr:uid="{33F28F8D-3FE9-4D0B-AAF5-92EAB42A7352}"/>
+    <hyperlink ref="G34" tooltip="Manufacturer" display="'CSD19502Q5B" xr:uid="{A85144DE-F884-4105-97AB-97F52013653B}"/>
+    <hyperlink ref="L34" tooltip="Supplier" display="'296-37194-1-ND" xr:uid="{3110E487-AA3A-445D-BF93-2AE3FF1357FF}"/>
+    <hyperlink ref="F35" tooltip="Component" display="'Yageo" xr:uid="{453A8C6C-C9D9-4354-8D54-67B5DE6A78B5}"/>
+    <hyperlink ref="G35" tooltip="Manufacturer" display="'RC0402JR-0710KL" xr:uid="{632DB630-60E8-4C25-B46D-3A0BD3DBE556}"/>
+    <hyperlink ref="L35" tooltip="Supplier" display="'311-10KJRTR-ND" xr:uid="{28F0FBC6-C0EC-4088-B8CF-C74ADC4B72B5}"/>
+    <hyperlink ref="F36" tooltip="Component" display="'Stackpole Electronics Inc." xr:uid="{2F338EA8-7C76-47B3-9836-42FBF53B3CF1}"/>
+    <hyperlink ref="G36" tooltip="Manufacturer" display="'CSNL2010FT1L00" xr:uid="{E37D2B7F-FEAD-4475-A777-2689A7572F9A}"/>
+    <hyperlink ref="L36" tooltip="Supplier" display="'CSNL2010FT1L00CT-ND" xr:uid="{649662FF-A7AB-414D-A587-51C87CD625FD}"/>
+    <hyperlink ref="F37" r:id="rId1" tooltip="Component" display="'" xr:uid="{E29193F0-ABEC-40CD-85D9-1C7D9EB81557}"/>
+    <hyperlink ref="G37" r:id="rId2" tooltip="Manufacturer" display="'" xr:uid="{22412495-F263-4B74-9B9B-1A614932A37D}"/>
+    <hyperlink ref="L37" r:id="rId3" tooltip="Supplier" display="'311-2.0KLRCT-ND" xr:uid="{348A5AC1-69F3-4892-AC38-A390838D36EC}"/>
+    <hyperlink ref="F38" tooltip="Component" display="'Vishay Dale" xr:uid="{E3AE608D-E1A4-4329-BD4E-66D17FF51850}"/>
+    <hyperlink ref="G38" tooltip="Manufacturer" display="'CRCW060328K0FKEA" xr:uid="{80ACBC77-9EE4-4542-9EAD-6B16088F6CDC}"/>
+    <hyperlink ref="L38" tooltip="Supplier" display="'541-28.0KHCT-ND" xr:uid="{AAF798A0-63F9-4012-8474-0155677B41D2}"/>
+    <hyperlink ref="F39" tooltip="Component" display="'Vishay Dale" xr:uid="{D47A8CB1-B919-443F-A76A-2D9C72F4E52E}"/>
+    <hyperlink ref="G39" tooltip="Manufacturer" display="'CRCW06038K45FKEA" xr:uid="{1EE091AB-F124-4526-9399-DA11D96F54DF}"/>
+    <hyperlink ref="L39" tooltip="Supplier" display="'541-8.45KHCT-ND" xr:uid="{01A44BB2-6620-492A-836C-05EDF0166CA2}"/>
+    <hyperlink ref="F40" tooltip="Component" display="'Yageo" xr:uid="{75C5E5F1-41C6-4198-8C1D-CE42E48DD3D7}"/>
+    <hyperlink ref="G40" tooltip="Manufacturer" display="'RC0805FR-0718KL" xr:uid="{A52F7DA9-BC85-4A60-A237-9382B13489AB}"/>
+    <hyperlink ref="L40" tooltip="Supplier" display="'311-18.0KCRCT-ND" xr:uid="{3F283A3F-7279-4F4E-AF89-09D073DD2140}"/>
+    <hyperlink ref="F41" tooltip="Component" display="'Yageo" xr:uid="{3DC7D7C0-B86C-442F-A968-BAAA9F063120}"/>
+    <hyperlink ref="G41" tooltip="Manufacturer" display="'RC0805FR-071KL" xr:uid="{6BCCABCB-855C-421B-A1A1-8159DCF21D94}"/>
+    <hyperlink ref="L41" tooltip="Supplier" display="'311-1.00KCRCT-ND" xr:uid="{F444B8F5-2FB3-4C8D-B4CA-B225922C0FE8}"/>
+    <hyperlink ref="F42" tooltip="Component" display="'Bourns Inc." xr:uid="{7B71876C-9274-46C4-A882-44676C9B8A39}"/>
+    <hyperlink ref="G42" tooltip="Manufacturer" display="'PWR163S-25-1R00J" xr:uid="{CB3E78F1-7A9C-4292-8D82-A4D41AFB898B}"/>
+    <hyperlink ref="L42" tooltip="Supplier" display="'PWR163S-25-1R00J-ND" xr:uid="{11FE0332-9B0E-46C6-88F8-DBF7691EBA0F}"/>
+    <hyperlink ref="F43" tooltip="Component" display="'Yageo" xr:uid="{8FED51FA-59B1-4AC9-88CD-538364B13A93}"/>
+    <hyperlink ref="G43" tooltip="Manufacturer" display="'RC0402FR-0710KL" xr:uid="{F6B0DB77-A5B6-4D3E-B93D-AAAEB00467DF}"/>
+    <hyperlink ref="L43" tooltip="Supplier" display="'311-10.0KLRCT-ND" xr:uid="{56D02BE6-5D65-4A72-9599-D92E58C389C0}"/>
+    <hyperlink ref="F44" tooltip="Component" display="'Samsung Electro-Mechanics America, Inc." xr:uid="{CDCD15C3-A89F-4BEC-879C-A6DDDE7DB5C2}"/>
+    <hyperlink ref="G44" tooltip="Manufacturer" display="'RC1005F102CS" xr:uid="{0CE3A6B0-587A-4546-AE0B-DC9D009C5E9F}"/>
+    <hyperlink ref="L44" tooltip="Supplier" display="'1276-3430-1-ND" xr:uid="{D6F414D3-FB37-4BB5-B63D-535653659DD1}"/>
+    <hyperlink ref="F45" tooltip="Component" display="'Yageo" xr:uid="{F4FDACDE-AB3D-4272-B819-30DC9EFCDD4F}"/>
+    <hyperlink ref="G45" tooltip="Manufacturer" display="'RC0402FR-07120RL" xr:uid="{093A065B-3744-41AB-A421-B539914AE48E}"/>
+    <hyperlink ref="L45" tooltip="Supplier" display="'311-120LRCT-ND" xr:uid="{5282B21E-7518-4356-9DEA-AC573F8EC684}"/>
+    <hyperlink ref="F46" tooltip="Component" display="'Panasonic Electronic Components" xr:uid="{DBFBF223-B8EA-4541-BD7F-FE2FCBED1583}"/>
+    <hyperlink ref="G46" tooltip="Manufacturer" display="'ERJ-1GN0R00C" xr:uid="{29DB9579-3A81-4878-9C9B-96844A507267}"/>
+    <hyperlink ref="L46" tooltip="Supplier" display="'P15979TR-ND" xr:uid="{9A5C94AF-35FB-42EB-8765-22098B382D96}"/>
+    <hyperlink ref="F47" tooltip="Component" display="'STMicroelectronics" xr:uid="{086C31C9-69B1-481F-B086-9885D03A3A4B}"/>
+    <hyperlink ref="G47" tooltip="Manufacturer" display="'VL53L0CXV0DH/1" xr:uid="{07C1C09F-DAB9-4B6F-96C0-A9D16967CD28}"/>
+    <hyperlink ref="L47" tooltip="Supplier" display="'497-16538-2-ND" xr:uid="{35467EE7-6906-46B2-B0FA-43A054AA3BE0}"/>
+    <hyperlink ref="F48" tooltip="Component" display="'Texas Instruments" xr:uid="{2FEBAF97-C911-415C-9F72-BCBF8C5BD3C1}"/>
+    <hyperlink ref="G48" tooltip="Manufacturer" display="'DRV8323RHRGZR" xr:uid="{706B7C63-F5CC-4E81-810E-B5E986A86AEB}"/>
+    <hyperlink ref="L48" tooltip="Supplier" display="'DRV8323RHRGZR-ND" xr:uid="{54E4EDE5-FE2E-484D-8C05-58D75AF815A2}"/>
+    <hyperlink ref="F49" tooltip="Component" display="'STMICROELECTRONICS" xr:uid="{E79ED518-7B52-45CD-A3FB-2E3382B11AB3}"/>
+    <hyperlink ref="G49" tooltip="Manufacturer" display="'STM32F769AIY6TR" xr:uid="{EDA9839E-DB86-40F1-BB9F-F6FE54BD6070}"/>
+    <hyperlink ref="L49" tooltip="Supplier" display="'84Y8745" xr:uid="{3803CD56-DC7A-451F-903B-67DACAB1FBEE}"/>
+    <hyperlink ref="F50" tooltip="Component" display="'NXP USA Inc." xr:uid="{CE73E80B-EBDE-441D-8955-7EAF993B537A}"/>
+    <hyperlink ref="G50" tooltip="Manufacturer" display="'TJA1052IT/5Y" xr:uid="{40A72EE1-10D9-4A69-8158-E7154CBA61A9}"/>
+    <hyperlink ref="L50" tooltip="Supplier" display="'568-11942-1-ND" xr:uid="{DCF5A66F-CC92-4F96-B4A2-671441F144B0}"/>
+    <hyperlink ref="F51" tooltip="Component" display="'Monolithic Power Systems Inc." xr:uid="{D7B724CE-6E02-43CD-B705-15A3361A3C8A}"/>
+    <hyperlink ref="G51" tooltip="Manufacturer" display="'MA700GQ-Z" xr:uid="{579A5C84-3F20-4AE2-85AB-7CF9A251116C}"/>
+    <hyperlink ref="L51" tooltip="Supplier" display="'MA700GQ-Z-ND" xr:uid="{DDAE1930-04CA-443B-B93C-C5E9E7358524}"/>
+    <hyperlink ref="F52" tooltip="Component" display="'Supplier disabled" xr:uid="{71A10B19-175F-40C4-8149-44BB27119D1C}"/>
+    <hyperlink ref="G52" tooltip="Manufacturer" display="'Supplier disabled" xr:uid="{B7D33F8A-831F-43DF-B1E6-8A472A6B7288}"/>
+    <hyperlink ref="L52" tooltip="Supplier" display="'Component Distributors Inc. - ICM-20649" xr:uid="{599976B8-96FF-4A12-BFF9-FCBDEB861A12}"/>
+    <hyperlink ref="F53" tooltip="Component" display="'ON Semiconductor" xr:uid="{93BA6F6F-C914-487A-ADF4-EC83603F1431}"/>
+    <hyperlink ref="G53" tooltip="Manufacturer" display="'NCV8154MTW180280TCG" xr:uid="{8A17B21B-D973-43A6-BD3E-E02D1DB85267}"/>
+    <hyperlink ref="L53" tooltip="Supplier" display="'NCV8154MTW180280TCGOSTR-ND" xr:uid="{FAA7721F-6CE5-4D11-8655-15D63CE0C060}"/>
+    <hyperlink ref="F54" tooltip="Component" display="'Linear Technology" xr:uid="{C4D19692-45C7-4B92-8033-E17AE1A7173C}"/>
+    <hyperlink ref="G54" tooltip="Manufacturer" display="'LTC4316IDD#PBF" xr:uid="{C3138BFD-309C-4BF3-B52A-EF5240FF49DB}"/>
+    <hyperlink ref="L54" tooltip="Supplier" display="'LTC4316IDD#PBF-ND" xr:uid="{25AE9708-847C-4D8E-A683-10D968895537}"/>
+    <hyperlink ref="F55" tooltip="Component" display="'TXC CORPORATION" xr:uid="{D45EF926-24DF-40FD-9CB6-4898D181F099}"/>
+    <hyperlink ref="G55" tooltip="Manufacturer" display="'8Q-24.000MEEV-T" xr:uid="{C15FAD55-40E7-4351-B5FD-82922000731B}"/>
+    <hyperlink ref="L55" tooltip="Supplier" display="'887-1846-2-ND" xr:uid="{008A0143-1050-4628-B9D0-C3E6F5A7E2C7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>